<commit_message>
Working on LM Sequencing Problem
</commit_message>
<xml_diff>
--- a/Rubric_project/Data/Learning_Materials_Base_set.xlsx
+++ b/Rubric_project/Data/Learning_Materials_Base_set.xlsx
@@ -3301,7 +3301,7 @@
     <t xml:space="preserve">https://avolve.apps.dso.mil/#/display/1b1b6490-c7c9-4cd9-b51c-c6bd4d672b39</t>
   </si>
   <si>
-    <t xml:space="preserve">Image Classification, Methods for explanation of AI results </t>
+    <t xml:space="preserve">Image Classification, Methods for explanation of AI results</t>
   </si>
   <si>
     <t xml:space="preserve">This article addresses the challenge of distinguishing between real photographs and those generated by AI, given the rise in synthetic data quality. It proposes a computer vision approach using a Convolutional Neural Network (CNN) to classify images as real or AI-generated, achieving an impressive accuracy of 92.98% after extensive training and optimization. Interestingly, the study finds that small imperfections in the background, rather than the main subject, are crucial for classification, shedding light on the model's decision-making process. The CIFAKE dataset, created for this research, is shared openly for further study in the field.</t>
@@ -4843,25 +4843,7 @@
     <t xml:space="preserve">https://avolve.apps.dso.mil/#/display/26bc4260-2913-4131-8ac6-8554d82b0f38</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Methods for explanation of AI results, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Supervised machine learning: symbolic models</t>
-    </r>
+    <t xml:space="preserve">Methods for explanation of AI results, Supervised machine learning: symbolic models</t>
   </si>
   <si>
     <t xml:space="preserve">Watch this episode of AI Explained to learn about AI reasoning, the cognitive process that enables AI to solve problems and think critically.</t>
@@ -5857,25 +5839,7 @@
     <t xml:space="preserve">https://avolve.apps.dso.mil/#/display/005cb895-7bdf-4613-b1e5-5e3a082f0837</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Required amount of data to adequately train a model, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Linear Models, Nonlinear models and artificial neural networks</t>
-    </r>
+    <t xml:space="preserve">Required amount of data to adequately train a model, Linear Models, Nonlinear models and artificial neural networks</t>
   </si>
   <si>
     <t xml:space="preserve">AI promises to touch every aspect of work and life, but how do they get made? In this video Martin keen walks through a five step framework for how to build and deploy AI models.</t>
@@ -6517,25 +6481,7 @@
     <t xml:space="preserve">https://avolve.apps.dso.mil/#/display/f8b52d25-2656-4de1-8e1c-d18c1044260f</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Supervised machine learning: numeric models, Supervised machine learning: symbolic models, Symbolic Reasoning, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Supervised and unsupervised learning</t>
-    </r>
+    <t xml:space="preserve">Supervised machine learning: numeric models, Supervised machine learning: symbolic models, Symbolic Reasoning, Supervised and unsupervised learning</t>
   </si>
   <si>
     <t xml:space="preserve">In this article, supervised learning is explained as a method of machine learning using labeled datasets to teach algorithms to make accurate predictions or classifications. Various algorithms and applications are discussed.</t>
@@ -6931,25 +6877,7 @@
     <t xml:space="preserve">https://avolve.apps.dso.mil/#/display/c1ccbbdf-1097-461a-bf78-ce7ced4606db</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rating employment contracts, Tracking contractor execution, Researching possible contracts, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">U.S. Government AI initiatives</t>
-    </r>
+    <t xml:space="preserve">Rating employment contracts, Tracking contractor execution, Researching possible contracts, U.S. Government AI initiatives</t>
   </si>
   <si>
     <t xml:space="preserve">This AI Guide for Government is intended to help government decision makers clearly see what AI means for their agencies and how to invest and build AI capabilities.</t>
@@ -7099,7 +7027,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -7137,12 +7065,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7206,7 +7128,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -7267,11 +7189,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7469,8 +7387,8 @@
   </sheetPr>
   <dimension ref="A1:AS1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A325" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B325" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A219" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A237" activeCellId="0" sqref="A237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32393,7 +32311,7 @@
       <c r="Y242" s="11" t="s">
         <v>1606</v>
       </c>
-      <c r="Z242" s="15" t="s">
+      <c r="Z242" s="7" t="s">
         <v>1607</v>
       </c>
       <c r="AA242" s="7" t="s">
@@ -37852,7 +37770,7 @@
       <c r="Y295" s="11" t="s">
         <v>1938</v>
       </c>
-      <c r="Z295" s="15" t="s">
+      <c r="Z295" s="7" t="s">
         <v>1939</v>
       </c>
       <c r="AA295" s="7" t="s">
@@ -42472,10 +42390,10 @@
       <c r="T340" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="U340" s="16" t="s">
+      <c r="U340" s="15" t="s">
         <v>2217</v>
       </c>
-      <c r="V340" s="16" t="s">
+      <c r="V340" s="15" t="s">
         <v>326</v>
       </c>
       <c r="W340" s="7" t="s">

</xml_diff>